<commit_message>
update normal mt case
</commit_message>
<xml_diff>
--- a/algieba/test/module_test.xlsx
+++ b/algieba/test/module_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -48,10 +48,6 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>条件</t>
     <rPh sb="0" eb="2">
       <t>ジョウケン</t>
@@ -59,104 +55,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>interval: 'monthly'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>interval: 'daily'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'income'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  date: Time.now.strftime('%Y-%m-%d')
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  content: 'テスト用データ'
-}</t>
-    <rPh sb="28" eb="29">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  category: 'テスト'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  price: 100
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'expense',
-  category: 'テスト'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'income'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  category: 'テスト'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  price: 100
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  date: Time.now.strftime('%Y-%m-%d'),
-  price: 100
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>interval: 'monthly'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>interval: 'daily'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>指定した条件のレコードが存在しない場合</t>
-    <rPh sb="0" eb="2">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ジョウケン</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ソンザイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>バアイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -226,69 +133,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[true, []]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[true, [&lt;検索結果&gt;]]</t>
-    <rPh sb="9" eb="13">
-      <t>ケンサクケッカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[true, [更新されたレコード]]</t>
-    <rPh sb="8" eb="10">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[true, []]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[true, []]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{&lt;期間&gt;: &lt;計算結果&gt;}</t>
-    <rPh sb="2" eb="4">
-      <t>キカン</t>
-    </rPh>
-    <rPh sb="8" eb="12">
-      <t>ケイサンケッカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  date: Time.now.strftime('%Y-%m-%d'),
-  price: 1
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  content: 'テスト用データ',
-  price: 100
-}</t>
-    <rPh sb="28" eb="29">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  content: 'テスト用データ',
-  price: 1
-}</t>
-    <rPh sb="28" eb="29">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>interval: 'yearly'</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -303,92 +147,6 @@
   account_type: 'invalid_type',
   date: Time.now.strftime('%Y-%m-%d'),
   price: 'invalid_value'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'expense'
-},
-with: {
-  account_type: 'income'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  date: Time.now.strftime('%Y-%m-%d')
-},
-with: {
-  date: Time.now.strftime('%Y-m-%d') &lt;&lt; 1
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  content: 'テスト用データ'
-},
-with: {
-  content: '更新後データ'
-}</t>
-    <rPh sb="28" eb="29">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="57" eb="60">
-      <t>コウシンゴ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  category: 'テスト'
-},
-with: {
-  category: '更新'
-}</t>
-    <rPh sb="55" eb="57">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  price: 100
-},
-with: {
-  price: 1000
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'expence',
-  price: 100
-},
-with: {
-  account_type: 'income',
-  category: 'テスト',
-  price: 10000
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'expence',
-  price: 1
-},
-with: {
-  account_type: 'income',
-  category: 'テスト',
-  price: 10000
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {},
-with: {
-  account_type: 'income',
-  price: 100000
 }</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -486,10 +244,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Account.show</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Account.destroy</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -498,7 +252,225 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Account.destroy</t>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_before: '1000-01-01'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_after: '1000-01-02'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  content_include: 'モジュールテスト'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  content_equal: 'モジュールテスト用データ1'
+ }</t>
+    <rPh sb="39" eb="40">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  category: 'algieba'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  price_upper: '100'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  price_lower: '100'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  account_type: 'income'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  account_type: 'expense',
+  category: 'algieba'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_before: '1000-01-01',
+  content_include: 'テスト'
+ }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  content_equal: 'モジュールテスト用データ2',
+  price_upper: '1000'
+ }</t>
+    <rPh sb="39" eb="40">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_after: '1000-01-01',
+  price_lower: '1000'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  account_type: 'income',
+  date_before: '1000-01-10',
+  date_after: '1000-01-01',
+  content_include: 'モジュールテスト',
+  category: 'algieba',
+  price_upper: '100',
+  price_lower: '1000'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下の家計簿がDBに登録されている
+{
+  account_type: 'income',
+  date: '1000-01-01',
+  content: 'モジュールテスト用データ1',
+  category: 'algieba',
+  price: 1000
+},
+{
+  account_type: 'expense',
+  date: '1000-01-05',
+  content: 'モジュールテスト用データ2',
+  category: 'algieba',
+  price: 100
+}</t>
+    <rPh sb="0" eb="2">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="207" eb="208">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{'1000': 900}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{'1000-01': 900}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  '1000-01-01': 1000,
+  '1000-01-05': -100
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[
+  {
+    account_type: 'income',
+    date: '1000-01-01',
+    content: 'モジュールテスト用データ1',
+    category: 'algieba',
+    price: 1000
+  }
+]</t>
+    <rPh sb="72" eb="81">
+      <t>モジュール</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[
+  {
+    account_type: 'expense',
+    date: '1000-01-05',
+    content: 'モジュールテスト用データ2',
+    category: 'algieba',
+    price: 100
+  }
+]</t>
+    <rPh sb="73" eb="82">
+      <t>モジュール</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[
+  {
+    account_type: 'income',
+    date: '1000-01-01',
+    content: 'モジュールテスト用データ1',
+    category: 'algieba',
+    price: 1000
+  },
+  {
+    account_type: 'expense',
+    date: '1000-01-05',
+    content: 'モジュールテスト用データ2',
+    category: 'algieba',
+    price: 100
+  }
+]</t>
+    <rPh sb="72" eb="81">
+      <t>モジュール</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -555,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -836,19 +808,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -857,6 +816,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1043,7 +1076,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1083,15 +1116,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1107,11 +1131,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="183">
@@ -1626,17 +1698,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G30"/>
+  <dimension ref="B1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="4" max="4" width="47.1640625" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col min="5" max="5" width="38.5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1655,13 +1727,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="44">
+    <row r="3" spans="2:7">
       <c r="B3" s="8">
         <v>1</v>
       </c>
@@ -1669,17 +1741,19 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>60</v>
+      </c>
       <c r="G3" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="44">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -1687,491 +1761,290 @@
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="32"/>
       <c r="G4" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="44">
-      <c r="B5" s="8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="57">
+      <c r="B5" s="24">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="44">
+      <c r="D5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="122">
       <c r="B6" s="8">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="44">
+      <c r="C6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="122">
       <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="57">
+      <c r="C7" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="122">
       <c r="B8" s="8">
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="57">
+      <c r="C8" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="122">
       <c r="B9" s="8">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="57">
+      <c r="C9" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="213">
       <c r="B10" s="8">
         <v>8</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="C10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="32"/>
+      <c r="G10" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="213">
       <c r="B11" s="8">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="83">
+      <c r="C11" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="213">
       <c r="B12" s="8">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="C12" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="83">
+      <c r="F12" s="32"/>
+      <c r="G12" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="122">
       <c r="B13" s="8">
         <v>11</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="C13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="83">
+      <c r="F13" s="32"/>
+      <c r="G13" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="122">
       <c r="B14" s="8">
         <v>12</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="83">
+      <c r="C14" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="122">
       <c r="B15" s="8">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="83">
+      <c r="C15" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="57">
       <c r="B16" s="8">
         <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="122">
+      <c r="C16" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="32"/>
+      <c r="G16" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="213">
       <c r="B17" s="8">
         <v>15</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13" t="s">
-        <v>40</v>
+      <c r="C17" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="37" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="122">
       <c r="B18" s="8">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="70">
-      <c r="B19" s="8">
+      <c r="C18" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="214" thickBot="1">
+      <c r="B19" s="15">
         <v>17</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="44">
-      <c r="B20" s="8">
-        <v>18</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="44">
-      <c r="B21" s="8">
-        <v>19</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13" t="s">
+      <c r="C19" s="30" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="44">
-      <c r="B22" s="8">
-        <v>20</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="44">
-      <c r="B23" s="8">
-        <v>21</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="44">
-      <c r="B24" s="8">
-        <v>22</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="57">
-      <c r="B25" s="8">
-        <v>23</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="57">
-      <c r="B26" s="8">
-        <v>24</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="11" t="s">
+      <c r="D19" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="8">
-        <v>25</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="8">
-        <v>26</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="8">
-        <v>27</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="19" thickBot="1">
-      <c r="B30" s="15">
-        <v>28</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19" t="s">
-        <v>43</v>
+      <c r="E19" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="33"/>
+      <c r="G19" s="39" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:F19"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2187,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2214,316 +2087,316 @@
         <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="44">
-      <c r="B3" s="20">
+      <c r="B3" s="17">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="44">
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="44">
-      <c r="B5" s="20">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="70">
-      <c r="B6" s="20">
+      <c r="B6" s="17">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="83">
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="83">
-      <c r="B8" s="20">
+      <c r="B8" s="17">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="83">
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="96">
-      <c r="B10" s="20">
+      <c r="B10" s="17">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="83">
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="83">
-      <c r="B12" s="20">
+      <c r="B12" s="17">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="83">
-      <c r="B13" s="20">
+      <c r="B13" s="17">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="109">
+      <c r="B14" s="17">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="109">
-      <c r="B14" s="20">
-        <v>12</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="44">
-      <c r="B15" s="20">
+      <c r="B15" s="17">
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="44">
-      <c r="B16" s="20">
+      <c r="B16" s="17">
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="44">
-      <c r="B17" s="20">
+      <c r="B17" s="17">
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="70">
-      <c r="B18" s="20">
+      <c r="B18" s="17">
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="20">
+      <c r="B19" s="17">
         <v>17</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>69</v>
+      <c r="C19" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="13" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="19" thickBot="1">
@@ -2533,15 +2406,15 @@
       <c r="C20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24" t="s">
-        <v>28</v>
+      <c r="D20" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update exception mt case
</commit_message>
<xml_diff>
--- a/algieba/test/module_test.xlsx
+++ b/algieba/test/module_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -67,188 +67,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>condition: {
-  account_type: 'invalid_type'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  price: -100
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'invalid_type'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'invalid_type',
-  date: 'invalid_date',
-  price: '100'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>nil</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>interval: 'invalid_interval'</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>nil</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>interval: nil</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[false, [:account_type]]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[false, [:date]]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[false, [:price]]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[false, [:account_type, :price]]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[false, [:account_type, :date]]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[false, [:account_type, :date]]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>interval: 'yearly'</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>condition: {
-  date: '1000-00-00'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'invalid_type',
-  date: Time.now.strftime('%Y-%m-%d'),
-  price: 'invalid_value'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'invalid_type
-},
-with: {
-  account_type: 'income'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  date: 'invalid_date'
-},
-with: {
-  category: 'テスト'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  price: 'invalid_price'
-}
-with: {
-  price: 100
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'income',
-  price: -100
-},
-with: {
-  account_type: 'expense'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'expense'
-},
-with: {
-  account_type: 'invalid_type'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  category: 'テスト'
-},
-with: {
-  date: 1000-00-00
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  price: 100
-},
-with: {
-  price: -100
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  account_type: 'income',
-  category: 'テスト'
-},
-with: {
-  account_type: 'invalid_type',
-  date: 'invalid_date'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>condition: {
-  date: '1000-00-00'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account.show</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account.update</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Account.settle</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account.destroy</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account.destroy</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -471,6 +302,167 @@
   </si>
   <si>
     <t>[]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  account_type: 'invalid_type'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_before: 'invalid_date_before'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_after: '01-01-1000'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_after: '1000-01-40'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  price_upper: 'invalid_price_upper'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  price_lower: '-100'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  price_lower: '100.0'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  account_type: 'invalid_type',
+  content_equal: 'モジュールテスト用データ1'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  date_after: '01-01-1000'
+  price_upper: '-100'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'account_type'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'date_before'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'date_after'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'price_upper'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'price_lower'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'account_type'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'date_after,price_upper'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  account_type: 'invalid_type',
+  date_before: 'invalid_date',
+  date_after: '1000-13-00',
+  price_upper: '-100',
+  price_lower: '0.0'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'account_type,date_before
+,date_after,price_upper,price_lower'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下の家計簿がDBに登録されている
+{
+  account_type: 'income',
+  date: '1000-01-01',
+  content: 'モジュールテスト用データ1',
+  category: 'algieba',
+  price: 1000
+},
+{
+  account_type: 'expense',
+  date: '1000-01-05',
+  content: 'モジュールテスト用データ2',
+  category: 'algieba',
+  price: 100
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'invalid'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArgumentError, :message =&gt; 'absent'</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -527,7 +519,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -652,7 +644,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -669,7 +663,24 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -682,8 +693,23 @@
       <right style="medium">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -692,116 +718,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -884,6 +804,17 @@
         <color auto="1"/>
       </left>
       <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
@@ -1076,77 +1007,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1155,35 +1065,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="183">
@@ -1726,7 +1663,7 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1734,311 +1671,311 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="57">
+      <c r="B5" s="17">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="122">
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="122">
+      <c r="B7" s="6">
+        <v>5</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="122">
+      <c r="B8" s="6">
+        <v>6</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="14" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="122">
+      <c r="B9" s="6">
+        <v>7</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="213">
+      <c r="B10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="213">
+      <c r="B11" s="6">
+        <v>9</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="213">
+      <c r="B12" s="6">
+        <v>10</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="122">
+      <c r="B13" s="6">
+        <v>11</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="57">
-      <c r="B5" s="24">
-        <v>3</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="26" t="s">
+    </row>
+    <row r="14" spans="2:7" ht="122">
+      <c r="B14" s="6">
+        <v>12</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="122">
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="122">
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="122">
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="122">
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="213">
-      <c r="B10" s="8">
-        <v>8</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="213">
-      <c r="B11" s="8">
-        <v>9</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="213">
-      <c r="B12" s="8">
-        <v>10</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="122">
-      <c r="B13" s="8">
-        <v>11</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="122">
-      <c r="B14" s="8">
-        <v>12</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="37" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="15" spans="2:7" ht="122">
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="37" t="s">
-        <v>64</v>
+      <c r="C15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="57">
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="38" t="s">
-        <v>67</v>
+      <c r="C16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="213">
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="37" t="s">
-        <v>66</v>
+      <c r="C17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="27" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="122">
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>16</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="37" t="s">
-        <v>64</v>
+      <c r="C18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="214" thickBot="1">
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <v>17</v>
       </c>
-      <c r="C19" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="39" t="s">
-        <v>66</v>
+      <c r="C19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="32"/>
+      <c r="G19" s="29" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2058,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G20"/>
+  <dimension ref="B1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2069,7 +2006,8 @@
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="4" max="4" width="47.1640625" customWidth="1"/>
     <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="7" width="47.1640625" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" customWidth="1"/>
+    <col min="7" max="7" width="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="19" thickBot="1"/>
@@ -2086,338 +2024,235 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="44">
-      <c r="B3" s="17">
+    <row r="3" spans="2:7">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="C3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="44">
+      <c r="F3" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4" s="17">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
-        <v>19</v>
+      <c r="D4" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="35" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="44">
-      <c r="B5" s="17">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="44">
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="44">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="C7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="44">
+      <c r="B8" s="6">
+        <v>6</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="44">
+      <c r="B9" s="6">
+        <v>7</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="44">
+      <c r="B10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="44">
+      <c r="B11" s="6">
+        <v>9</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="57">
+      <c r="B12" s="6">
+        <v>10</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="57">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="70">
-      <c r="B6" s="17">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="83">
-      <c r="B7" s="17">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="83">
-      <c r="B8" s="17">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="83">
-      <c r="B9" s="17">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="96">
-      <c r="B10" s="17">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="83">
-      <c r="B11" s="17">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="83">
-      <c r="B12" s="17">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="83">
-      <c r="B13" s="17">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="109">
-      <c r="B14" s="17">
+      <c r="C13" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="97" thickBot="1">
+      <c r="B14" s="12">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="44">
-      <c r="B15" s="17">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="44">
-      <c r="B16" s="17">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="44">
-      <c r="B17" s="17">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="70">
-      <c r="B18" s="17">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="17">
-        <v>17</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="19" thickBot="1">
-      <c r="B20" s="15">
-        <v>18</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21" t="s">
-        <v>14</v>
+      <c r="C14" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="41" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:F14"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
update normal ft case
</commit_message>
<xml_diff>
--- a/algieba/test/module_test.xlsx
+++ b/algieba/test/module_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -213,28 +213,6 @@
   '1000-01-01': 1000,
   '1000-01-05': -100
 }</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[
-  {
-    account_type: 'income',
-    date: '1000-01-01',
-    content: 'モジュールテスト用データ1',
-    category: 'algieba',
-    price: 1000
-  },
-  {
-    account_type: 'expense',
-    date: '1000-01-05',
-    content: 'モジュールテスト用データ2',
-    category: 'algieba',
-    price: 100
-  }
-]</t>
-    <rPh sb="72" eb="81">
-      <t>モジュール</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1714,7 +1692,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>33</v>
@@ -1771,7 +1749,7 @@
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="135">
@@ -1789,7 +1767,7 @@
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="135">
@@ -1807,7 +1785,7 @@
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="135">
@@ -1825,10 +1803,10 @@
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="213">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="239">
       <c r="B10" s="6">
         <v>8</v>
       </c>
@@ -1843,10 +1821,10 @@
       </c>
       <c r="F10" s="40"/>
       <c r="G10" s="27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="213">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="239">
       <c r="B11" s="6">
         <v>9</v>
       </c>
@@ -1861,10 +1839,10 @@
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="213">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="239">
       <c r="B12" s="6">
         <v>10</v>
       </c>
@@ -1879,7 +1857,7 @@
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="27" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="135">
@@ -1897,7 +1875,7 @@
       </c>
       <c r="F13" s="40"/>
       <c r="G13" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="135">
@@ -1915,7 +1893,7 @@
       </c>
       <c r="F14" s="40"/>
       <c r="G14" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="135">
@@ -1933,7 +1911,7 @@
       </c>
       <c r="F15" s="40"/>
       <c r="G15" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="57">
@@ -1951,7 +1929,7 @@
       </c>
       <c r="F16" s="40"/>
       <c r="G16" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="239">
@@ -1969,7 +1947,7 @@
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="135">
@@ -1987,7 +1965,7 @@
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="240" thickBot="1">
@@ -2005,7 +1983,7 @@
       </c>
       <c r="F19" s="41"/>
       <c r="G19" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2075,10 +2053,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -2096,7 +2074,7 @@
       </c>
       <c r="F4" s="40"/>
       <c r="G4" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="44">
@@ -2104,17 +2082,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="40"/>
       <c r="G5" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="44">
@@ -2122,17 +2100,17 @@
         <v>4</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="44">
@@ -2140,17 +2118,17 @@
         <v>5</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="44">
@@ -2158,17 +2136,17 @@
         <v>6</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="44">
@@ -2176,17 +2154,17 @@
         <v>7</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="44">
@@ -2194,17 +2172,17 @@
         <v>8</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="40"/>
       <c r="G10" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="44">
@@ -2212,17 +2190,17 @@
         <v>9</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="57">
@@ -2230,17 +2208,17 @@
         <v>10</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="57">
@@ -2248,17 +2226,17 @@
         <v>11</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="40"/>
       <c r="G13" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="97" thickBot="1">
@@ -2266,17 +2244,17 @@
         <v>12</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>